<commit_message>
Add pred generation pipeline and classification report pipeline
</commit_message>
<xml_diff>
--- a/data/pred/ano_CV DE GABRIAC Jérôme.xlsx
+++ b/data/pred/ano_CV DE GABRIAC Jérôme.xlsx
@@ -108,8 +108,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="-1555115906281846638" xfId="1" hidden="0"/>
-    <cellStyle name="-9173829531760542027" xfId="2" hidden="0"/>
+    <cellStyle name="-573996148845870281" xfId="1" hidden="0"/>
+    <cellStyle name="6016113629736608966" xfId="2" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>